<commit_message>
Added possibility to provide several Scenario Outlines in one feature. Data are split in different outlines from a unique input file.
</commit_message>
<xml_diff>
--- a/src/test/resources/data/in/blog.xlsx
+++ b/src/test/resources/data/in/blog.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2445" windowWidth="14670" windowHeight="5745"/>
@@ -189,6 +189,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -236,7 +239,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -271,7 +274,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -480,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,47 +576,51 @@
       <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E6" s="11">
         <v>2</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F6" s="12">
         <v>3</v>
       </c>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E7" s="7">
         <v>9</v>
       </c>
-      <c r="F6" s="8"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
@@ -665,6 +672,7 @@
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
@@ -746,6 +754,9 @@
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B48" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Brought modifications in counters to work with multiple scenarios features
</commit_message>
<xml_diff>
--- a/src/test/resources/data/in/blog.xlsx
+++ b/src/test/resources/data/in/blog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14670" windowHeight="5745"/>
+    <workbookView xWindow="0" yWindow="2448" windowWidth="14676" windowHeight="5748"/>
   </bookViews>
   <sheets>
     <sheet name="NoraUi-blog" sheetId="1" r:id="rId1"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -486,19 +486,19 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.5546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>16</v>
       </c>
@@ -518,7 +518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -537,7 +537,7 @@
       <c r="F2" s="5"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -556,7 +556,7 @@
       <c r="F3" s="8"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -575,7 +575,7 @@
       <c r="F4" s="8"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -583,7 +583,7 @@
       <c r="F5" s="8"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>18</v>
       </c>
@@ -604,7 +604,7 @@
       </c>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -622,140 +622,140 @@
       </c>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B31" s="1"/>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B32" s="1"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" s="1"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" s="1"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" s="1"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" s="1"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B38" s="1"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39" s="1"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B40" s="1"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B41" s="1"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B42" s="1"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B43" s="1"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B44" s="1"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B45" s="1"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B46" s="1"/>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B47" s="1"/>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B48" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
use blog in English and fix all CI/CD data
</commit_message>
<xml_diff>
--- a/src/test/resources/data/in/blog.xlsx
+++ b/src/test/resources/data/in/blog.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2448" windowWidth="14676" windowHeight="5748"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14670" windowHeight="5745"/>
   </bookViews>
   <sheets>
     <sheet name="NoraUi-blog" sheetId="1" r:id="rId1"/>
@@ -19,18 +19,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
-    <t>Résultat</t>
-  </si>
-  <si>
-    <t>Titre</t>
-  </si>
-  <si>
-    <t>Texte</t>
-  </si>
-  <si>
-    <t>Auteur</t>
-  </si>
-  <si>
     <t>Note</t>
   </si>
   <si>
@@ -77,12 +65,24 @@
   </si>
   <si>
     <t>anonymous</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Result</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -239,7 +239,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -274,7 +274,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -486,50 +486,50 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="C1" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E2" s="6">
         <v>7</v>
@@ -537,18 +537,18 @@
       <c r="F2" s="5"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="E3" s="7">
         <v>10</v>
@@ -556,18 +556,18 @@
       <c r="F3" s="8"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E4" s="7">
         <v>8</v>
@@ -575,7 +575,7 @@
       <c r="F4" s="8"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -583,18 +583,18 @@
       <c r="F5" s="8"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E6" s="11">
         <v>2</v>
@@ -604,158 +604,158 @@
       </c>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E7" s="7">
         <v>9</v>
       </c>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B31" s="1"/>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B32" s="1"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B34" s="1"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B35" s="1"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B36" s="1"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B37" s="1"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B38" s="1"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B39" s="1"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B40" s="1"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B41" s="1"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" s="1"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
     </row>
   </sheetData>

</xml_diff>